<commit_message>
[Edit] - Remove back btn on appbar
</commit_message>
<xml_diff>
--- a/output/Notepad output.xlsx
+++ b/output/Notepad output.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development - flutter\FF-R02_Notepad\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1284B065-DD30-4A63-99C4-21CFB891C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9160DFB4-AE50-489F-8DCB-4EFEDF19A03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
     <sheet name="Add Note" sheetId="2" r:id="rId2"/>
     <sheet name="Display all notes" sheetId="3" r:id="rId3"/>
+    <sheet name="Remove back btn" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,9 +27,18 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Remove back button on appbar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +48,22 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -64,8 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,6 +423,99 @@
         <a:xfrm>
           <a:off x="670560" y="457200"/>
           <a:ext cx="4295238" cy="8390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>549016</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>396240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>98512</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>395178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAD0AE29-F1D7-92BA-369D-19A92B08DEAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="549016" y="1005840"/>
+          <a:ext cx="4243416" cy="8228538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1356</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>138002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF0BA1D-49C8-DC59-C621-902411BD92A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5669280" y="883920"/>
+          <a:ext cx="4390476" cy="8504762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -704,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02107DE-405E-4C6F-978B-477F0FEFDED1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -714,4 +835,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360BC207-B0E5-454B-A541-D98E392E9BB4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>